<commit_message>
few changes and scrum details in case study folder
</commit_message>
<xml_diff>
--- a/Case Study/Sample_Retrospective Backlog.xlsx
+++ b/Case Study/Sample_Retrospective Backlog.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\D-Drive\CDEG\Stream - Agile\ILP\Case Study_ILP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\data\python\royal bank\retail_bank\Case Study\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39E47879-F4D2-456E-B3D8-6BB94F388774}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
+    <workbookView xWindow="-132" yWindow="-132" windowWidth="23304" windowHeight="12624" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>The Good</t>
   </si>
@@ -41,11 +42,23 @@
   <si>
     <t>Start Doing - Improvement items/ Agreements on new way of working</t>
   </si>
+  <si>
+    <t>the coding is done at good pace and keep up</t>
+  </si>
+  <si>
+    <t>versioning isssues with git</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stop pushing to master directly </t>
+  </si>
+  <si>
+    <t>not using branches for versioning</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="[$-409]General"/>
     <numFmt numFmtId="165" formatCode="&quot; $&quot;#,##0.00&quot; &quot;;&quot; $(&quot;#,##0.00&quot;)&quot;;&quot; $-&quot;#&quot; &quot;;@&quot; &quot;"/>
@@ -495,6 +508,42 @@
     <xf numFmtId="0" fontId="14" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -525,182 +574,34 @@
     <xf numFmtId="0" fontId="13" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="24">
-    <cellStyle name="%" xfId="1"/>
-    <cellStyle name="_Q4 CC Business Scenarios" xfId="2"/>
-    <cellStyle name="Currency 2" xfId="3"/>
-    <cellStyle name="Excel Built-in Bad" xfId="4"/>
-    <cellStyle name="Excel Built-in Good" xfId="5"/>
-    <cellStyle name="Graphics" xfId="6"/>
-    <cellStyle name="Heading" xfId="7"/>
-    <cellStyle name="Heading1" xfId="8"/>
-    <cellStyle name="Hyperlink 2" xfId="9"/>
+    <cellStyle name="%" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="_Q4 CC Business Scenarios" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Currency 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Excel Built-in Bad" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Excel Built-in Good" xfId="5" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Graphics" xfId="6" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Heading" xfId="7" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Heading1" xfId="8" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Hyperlink 2" xfId="9" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="10"/>
-    <cellStyle name="Normal 2 2" xfId="11"/>
-    <cellStyle name="Normal 2 2 2" xfId="12"/>
-    <cellStyle name="Normal 2 3" xfId="13"/>
-    <cellStyle name="Normal 3" xfId="14"/>
-    <cellStyle name="Normal 4" xfId="15"/>
-    <cellStyle name="Normal 5" xfId="16"/>
-    <cellStyle name="Normal 6" xfId="17"/>
-    <cellStyle name="Normal 7" xfId="18"/>
-    <cellStyle name="Normal 7 2" xfId="19"/>
-    <cellStyle name="Percent 2" xfId="20"/>
-    <cellStyle name="Result" xfId="21"/>
-    <cellStyle name="Result2" xfId="22"/>
-    <cellStyle name="Style 1" xfId="23"/>
+    <cellStyle name="Normal 2" xfId="10" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="Normal 2 2" xfId="11" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
+    <cellStyle name="Normal 2 2 2" xfId="12" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
+    <cellStyle name="Normal 2 3" xfId="13" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
+    <cellStyle name="Normal 3" xfId="14" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
+    <cellStyle name="Normal 4" xfId="15" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
+    <cellStyle name="Normal 5" xfId="16" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
+    <cellStyle name="Normal 6" xfId="17" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
+    <cellStyle name="Normal 7" xfId="18" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
+    <cellStyle name="Normal 7 2" xfId="19" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
+    <cellStyle name="Percent 2" xfId="20" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
+    <cellStyle name="Result" xfId="21" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
+    <cellStyle name="Result2" xfId="22" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
+    <cellStyle name="Style 1" xfId="23" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
   </cellStyles>
-  <dxfs count="52">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="26"/>
-          <bgColor indexed="43"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="27"/>
-          <bgColor indexed="42"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="26"/>
-          <bgColor indexed="43"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="27"/>
-          <bgColor indexed="42"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="26"/>
-          <bgColor indexed="43"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="27"/>
-          <bgColor indexed="42"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="26"/>
-          <bgColor indexed="43"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="27"/>
-          <bgColor indexed="42"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="26"/>
-          <bgColor indexed="43"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="27"/>
-          <bgColor indexed="42"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="26"/>
-          <bgColor indexed="43"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="27"/>
-          <bgColor indexed="42"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="26"/>
-          <bgColor indexed="43"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="27"/>
-          <bgColor indexed="42"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="38">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1094,6 +995,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1129,6 +1047,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1304,259 +1239,272 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q5" sqref="Q5"/>
+      <selection activeCell="C11" sqref="C11:L11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="21"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="21.6"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" style="1"/>
-    <col min="5" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="20.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="9.109375" style="1"/>
+    <col min="5" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" ht="21.75" thickBot="1"/>
-    <row r="2" spans="2:12" ht="21.75" thickBot="1">
-      <c r="B2" s="4" t="s">
+    <row r="1" spans="2:12" ht="22.2" thickBot="1"/>
+    <row r="2" spans="2:12" ht="22.2" thickBot="1">
+      <c r="B2" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="6"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="18"/>
     </row>
     <row r="3" spans="2:12">
-      <c r="B3" s="7"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="9"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="20"/>
+      <c r="L3" s="21"/>
     </row>
     <row r="4" spans="2:12">
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="24"/>
-      <c r="J4" s="24"/>
-      <c r="K4" s="24"/>
-      <c r="L4" s="25"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="15"/>
     </row>
     <row r="5" spans="2:12">
-      <c r="B5" s="19"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="11"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="22"/>
+      <c r="J5" s="22"/>
+      <c r="K5" s="22"/>
+      <c r="L5" s="23"/>
     </row>
     <row r="6" spans="2:12">
-      <c r="B6" s="19"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="11"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="22"/>
+      <c r="K6" s="22"/>
+      <c r="L6" s="23"/>
     </row>
     <row r="7" spans="2:12">
-      <c r="B7" s="20"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="11"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="22"/>
+      <c r="J7" s="22"/>
+      <c r="K7" s="22"/>
+      <c r="L7" s="23"/>
     </row>
     <row r="8" spans="2:12" ht="6.75" customHeight="1">
       <c r="B8" s="3"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="12"/>
-      <c r="L8" s="13"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="24"/>
+      <c r="J8" s="24"/>
+      <c r="K8" s="24"/>
+      <c r="L8" s="25"/>
     </row>
     <row r="9" spans="2:12" ht="21" customHeight="1">
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="C9" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="24"/>
-      <c r="E9" s="24"/>
-      <c r="F9" s="24"/>
-      <c r="G9" s="24"/>
-      <c r="H9" s="24"/>
-      <c r="I9" s="24"/>
-      <c r="J9" s="24"/>
-      <c r="K9" s="24"/>
-      <c r="L9" s="25"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="15"/>
     </row>
     <row r="10" spans="2:12">
-      <c r="B10" s="19"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
-      <c r="L10" s="11"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="22"/>
+      <c r="L10" s="23"/>
     </row>
     <row r="11" spans="2:12">
-      <c r="B11" s="19"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="10"/>
-      <c r="K11" s="10"/>
-      <c r="L11" s="11"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="22"/>
+      <c r="K11" s="22"/>
+      <c r="L11" s="23"/>
     </row>
     <row r="12" spans="2:12">
-      <c r="B12" s="20"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="10"/>
-      <c r="L12" s="11"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="22"/>
+      <c r="K12" s="22"/>
+      <c r="L12" s="23"/>
     </row>
     <row r="13" spans="2:12" ht="6.75" customHeight="1">
       <c r="B13" s="3"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="12"/>
-      <c r="K13" s="12"/>
-      <c r="L13" s="13"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="24"/>
+      <c r="I13" s="24"/>
+      <c r="J13" s="24"/>
+      <c r="K13" s="24"/>
+      <c r="L13" s="25"/>
     </row>
     <row r="14" spans="2:12" ht="21" customHeight="1">
-      <c r="B14" s="21" t="s">
+      <c r="B14" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C14" s="24" t="s">
+      <c r="C14" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="D14" s="24"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="24"/>
-      <c r="H14" s="24"/>
-      <c r="I14" s="24"/>
-      <c r="J14" s="24"/>
-      <c r="K14" s="24"/>
-      <c r="L14" s="25"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="15"/>
     </row>
     <row r="15" spans="2:12">
-      <c r="B15" s="22"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="16"/>
-      <c r="J15" s="16"/>
-      <c r="K15" s="16"/>
-      <c r="L15" s="17"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="7"/>
     </row>
     <row r="16" spans="2:12">
-      <c r="B16" s="22"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="16"/>
-      <c r="H16" s="16"/>
-      <c r="I16" s="16"/>
-      <c r="J16" s="16"/>
-      <c r="K16" s="16"/>
-      <c r="L16" s="17"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="7"/>
     </row>
     <row r="17" spans="2:12">
-      <c r="B17" s="22"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="16"/>
-      <c r="H17" s="16"/>
-      <c r="I17" s="16"/>
-      <c r="J17" s="16"/>
-      <c r="K17" s="16"/>
-      <c r="L17" s="17"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="7"/>
     </row>
-    <row r="18" spans="2:12" ht="21.75" thickBot="1">
-      <c r="B18" s="23"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="14"/>
-      <c r="K18" s="14"/>
-      <c r="L18" s="15"/>
+    <row r="18" spans="2:12" ht="22.2" thickBot="1">
+      <c r="B18" s="13"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="B2:L3"/>
+    <mergeCell ref="C4:L4"/>
+    <mergeCell ref="C5:L5"/>
+    <mergeCell ref="C6:L6"/>
+    <mergeCell ref="C7:L7"/>
     <mergeCell ref="C18:L18"/>
     <mergeCell ref="C15:L15"/>
     <mergeCell ref="C16:L16"/>
@@ -1565,11 +1513,6 @@
     <mergeCell ref="B9:B12"/>
     <mergeCell ref="B14:B18"/>
     <mergeCell ref="C14:L14"/>
-    <mergeCell ref="B2:L3"/>
-    <mergeCell ref="C4:L4"/>
-    <mergeCell ref="C5:L5"/>
-    <mergeCell ref="C6:L6"/>
-    <mergeCell ref="C7:L7"/>
     <mergeCell ref="C8:L8"/>
     <mergeCell ref="C9:L9"/>
     <mergeCell ref="C10:L10"/>
@@ -1578,154 +1521,154 @@
     <mergeCell ref="C13:L13"/>
   </mergeCells>
   <conditionalFormatting sqref="D10:H12 D18:L18 D4:L8 I10:L10 B4 C15:L15 B8:B9">
-    <cfRule type="expression" dxfId="51" priority="43" stopIfTrue="1">
+    <cfRule type="expression" dxfId="37" priority="43" stopIfTrue="1">
       <formula>$D4="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="50" priority="44" stopIfTrue="1">
+    <cfRule type="expression" dxfId="36" priority="44" stopIfTrue="1">
       <formula>$D4="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I11:L12">
-    <cfRule type="expression" dxfId="49" priority="45" stopIfTrue="1">
+    <cfRule type="expression" dxfId="35" priority="45" stopIfTrue="1">
       <formula>$D11="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="48" priority="46" stopIfTrue="1">
+    <cfRule type="expression" dxfId="34" priority="46" stopIfTrue="1">
       <formula>$D11="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:C8">
-    <cfRule type="expression" dxfId="47" priority="47" stopIfTrue="1">
+    <cfRule type="expression" dxfId="33" priority="47" stopIfTrue="1">
       <formula>$D4="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="46" priority="48" stopIfTrue="1">
+    <cfRule type="expression" dxfId="32" priority="48" stopIfTrue="1">
       <formula>$D4="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="expression" dxfId="45" priority="49" stopIfTrue="1">
+    <cfRule type="expression" dxfId="31" priority="49" stopIfTrue="1">
       <formula>$D2="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="44" priority="50" stopIfTrue="1">
+    <cfRule type="expression" dxfId="30" priority="50" stopIfTrue="1">
       <formula>$D2="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="expression" dxfId="43" priority="51" stopIfTrue="1">
+    <cfRule type="expression" dxfId="29" priority="51" stopIfTrue="1">
       <formula>$D10="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="52" stopIfTrue="1">
+    <cfRule type="expression" dxfId="28" priority="52" stopIfTrue="1">
       <formula>$D10="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11">
-    <cfRule type="expression" dxfId="41" priority="53" stopIfTrue="1">
+    <cfRule type="expression" dxfId="27" priority="53" stopIfTrue="1">
       <formula>$D11="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="54" stopIfTrue="1">
+    <cfRule type="expression" dxfId="26" priority="54" stopIfTrue="1">
       <formula>$D11="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12">
-    <cfRule type="expression" dxfId="39" priority="55" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="55" stopIfTrue="1">
       <formula>$D12="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="38" priority="56" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="56" stopIfTrue="1">
       <formula>$D12="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18">
-    <cfRule type="expression" dxfId="37" priority="59" stopIfTrue="1">
+    <cfRule type="expression" dxfId="23" priority="59" stopIfTrue="1">
       <formula>$D18="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="60" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="60" stopIfTrue="1">
       <formula>$D18="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D17:L17">
-    <cfRule type="expression" dxfId="35" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="21" stopIfTrue="1">
       <formula>$D17="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="20" priority="22" stopIfTrue="1">
       <formula>$D17="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17">
-    <cfRule type="expression" dxfId="31" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="25" stopIfTrue="1">
       <formula>$D17="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="26" stopIfTrue="1">
       <formula>$D17="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D16:L16">
-    <cfRule type="expression" dxfId="29" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="15" stopIfTrue="1">
       <formula>$D16="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="16" stopIfTrue="1">
       <formula>$D16="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16">
-    <cfRule type="expression" dxfId="25" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="19" stopIfTrue="1">
       <formula>$D16="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="20" stopIfTrue="1">
       <formula>$D16="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="expression" dxfId="23" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="13" stopIfTrue="1">
       <formula>$D14="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="14" stopIfTrue="1">
       <formula>$D14="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D13:L13 B13">
-    <cfRule type="expression" dxfId="21" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="9" stopIfTrue="1">
       <formula>$D13="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="10" stopIfTrue="1">
       <formula>$D13="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13">
-    <cfRule type="expression" dxfId="19" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="11" stopIfTrue="1">
       <formula>$D13="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="12" stopIfTrue="1">
       <formula>$D13="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D14:L14">
-    <cfRule type="expression" dxfId="15" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="5" stopIfTrue="1">
       <formula>$D14="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="6" stopIfTrue="1">
       <formula>$D14="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14">
-    <cfRule type="expression" dxfId="11" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="7" stopIfTrue="1">
       <formula>$D14="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="8" stopIfTrue="1">
       <formula>$D14="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9:L9">
-    <cfRule type="expression" dxfId="7" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="1" stopIfTrue="1">
       <formula>$D9="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="2" stopIfTrue="1">
       <formula>$D9="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="expression" dxfId="3" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="3" stopIfTrue="1">
       <formula>$D9="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="4" stopIfTrue="1">
       <formula>$D9="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>